<commit_message>
Finish8ed all the main Questions
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\Documents\da11\excel\lookups-exercise-derekbeistad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61BE702-94F6-4AD2-A8B4-87D9F182DBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4499D8A-77D3-4253-A470-4DEEFAE9444D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21626" yWindow="-10697" windowWidth="21712" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25294" yWindow="-10697" windowWidth="25380" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -649,7 +649,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -764,6 +764,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -809,7 +824,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -821,6 +836,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -877,6 +893,985 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>metro_budget!$B$82</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>'Public Defender' Department Budget vs. Actual by Year</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8135400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8560800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8497500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A71-4C0B-B962-876DAFBEED80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7968645.8300000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8171472.0199999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8150982.5699999901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A71-4C0B-B962-876DAFBEED80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="287448895"/>
+        <c:axId val="1812529903"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="287448895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1812529903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1812529903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="287448895"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>54430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1681842</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>70757</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C975CE-181D-7227-A50F-98A1418AF039}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4623,12 +5618,19 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B82" t="str">
+        <f xml:space="preserve"> "'" &amp; A83 &amp; "' Department Budget vs. Actual by Year"</f>
+        <v>'Public Defender' Department Budget vs. Actual by Year</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A83" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -4636,26 +5638,44 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
+      <c r="B84" s="6">
+        <f>INDEX(B$2:B$52, MATCH($A$83,$A$2:$A$52,0))</f>
+        <v>8135400</v>
+      </c>
+      <c r="C84" s="6">
+        <f>INDEX(C$2:C$52, MATCH($A$83,$A$2:$A$52,0))</f>
+        <v>7968645.8300000001</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
+      <c r="B85" s="6">
+        <f>INDEX(G$2:G$52, MATCH($A$83,$A$2:$A$52,0))</f>
+        <v>8560800</v>
+      </c>
+      <c r="C85" s="6">
+        <f>INDEX(H$2:H$52, MATCH($A$83,$A$2:$A$52,0))</f>
+        <v>8171472.0199999996</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
+      <c r="B86" s="6">
+        <f>INDEX(L$2:L$52, MATCH($A$83,$A$2:$A$52,0))</f>
+        <v>8497500</v>
+      </c>
+      <c r="C86" s="6">
+        <f>INDEX(M$2:M$52, MATCH($A$83,$A$2:$A$52,0))</f>
+        <v>8150982.5699999901</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="7" t="s">
@@ -4792,12 +5812,13 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Choose Dept." prompt="Choose dept." sqref="A83" xr:uid="{7B728526-F4FC-424C-B19C-0659E0091209}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Working on Bonus Qs
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\Documents\da11\excel\lookups-exercise-derekbeistad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4499D8A-77D3-4253-A470-4DEEFAE9444D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED022DDB-C1A4-4AB8-9BB3-FA548B068EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25294" yWindow="-10697" windowWidth="25380" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24214" yWindow="-10697" windowWidth="24300" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -921,6 +921,14 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15071637481026248"/>
+          <c:y val="5.8542650197457968E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -934,7 +942,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1837,16 +1845,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>54430</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>40137</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1681842</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>620485</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>70757</xdr:rowOff>
+      <xdr:rowOff>178248</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2173,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5268,6 +5276,15 @@
       <c r="D55" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
@@ -5285,21 +5302,45 @@
         <f>VLOOKUP($A56, $A$1:$P$52, 14, FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
+      <c r="E56">
+        <f>VLOOKUP($A56, $A$1:$P$52, MATCH(E$55,$A$1:$P$1, 0), FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="F56">
+        <f t="shared" ref="F56:G56" si="9">VLOOKUP($A56, $A$1:$P$52, MATCH(F$55,$A$1:$P$1, 0), FALSE)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="9"/>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="9">VLOOKUP($A57, A2:P53, 4, FALSE)</f>
+        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A57, A2:P53, 4, FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="10">VLOOKUP($A57, $A$1:$P$52, 9, FALSE)</f>
+        <f t="shared" ref="C57:C61" si="11">VLOOKUP($A57, $A$1:$P$52, 9, FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="11">VLOOKUP($A57, $A$1:$P$52, 14, FALSE)</f>
+        <f t="shared" ref="D57:D61" si="12">VLOOKUP($A57, $A$1:$P$52, 14, FALSE)</f>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:G61" si="13">VLOOKUP($A57, $A$1:$P$52, MATCH(E$55,$A$1:$P$1, 0), FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="13"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5308,15 +5349,27 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="13"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="13"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="13"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5325,15 +5378,27 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="13"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="13"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="13"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5342,15 +5407,27 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="13"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="13"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="13"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5359,15 +5436,27 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="13"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="13"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="13"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5389,8 +5478,17 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5407,97 +5505,97 @@
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP($A66, $A$2:$A$52, $D$2:$D$52)</f>
+        <f t="shared" ref="B66:B70" si="14">_xlfn.XLOOKUP($A66, $A$2:$A$52, $D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP($A66, $A$2:$A$52, $I$2:$I$52)</f>
+        <f t="shared" ref="C66:C70" si="15">_xlfn.XLOOKUP($A66, $A$2:$A$52, $I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP($A66, $A$2:$A$52, $N$2:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="16">_xlfn.XLOOKUP($A66, $A$2:$A$52, $N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -5510,8 +5608,17 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -5527,89 +5634,161 @@
         <f>INDEX($N$2:$N$52, MATCH($A74, $A$2:$A$52, 0))</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E74">
+        <f>INDEX($A$2:$P$52,MATCH($A74,$A$2:$A$52,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="F74">
+        <f t="shared" ref="F74:G74" si="17">INDEX($A$2:$P$52,MATCH($A74,$A$2:$A$52,0),MATCH(F$73,$A$1:$P$1,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="17"/>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="15">INDEX($D$2:$D$52, MATCH($A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="B75:B79" si="18">INDEX($D$2:$D$52, MATCH($A75, $A$2:$A$52, 0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="16">INDEX($I$2:$I$52, MATCH($A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="C75:C79" si="19">INDEX($I$2:$I$52, MATCH($A75, $A$2:$A$52, 0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="17">INDEX($N$2:$N$52, MATCH($A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="D75:D79" si="20">INDEX($N$2:$N$52, MATCH($A75, $A$2:$A$52, 0))</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E75">
+        <f t="shared" ref="E75:G79" si="21">INDEX($A$2:$P$52,MATCH($A75,$A$2:$A$52,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="21"/>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E76">
+        <f t="shared" si="21"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="21"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="21"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E77">
+        <f t="shared" si="21"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="21"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="21"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E78">
+        <f t="shared" si="21"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="21"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="21"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="21"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="21"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="21"/>
         <v>-82077.349999999627</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished all main questions. Halfway throug Q8
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\Documents\da11\excel\lookups-exercise-derekbeistad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED022DDB-C1A4-4AB8-9BB3-FA548B068EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077386C2-F2EF-44B2-AF2D-0FE220890BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24214" yWindow="-10697" windowWidth="24300" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24900" yWindow="-10697" windowWidth="24986" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
@@ -314,7 +336,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +482,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -824,7 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -837,6 +865,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2181,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5488,7 +5517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5504,8 +5533,20 @@
         <f>_xlfn.XLOOKUP($A65, $A$2:$A$52, $N$2:$N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E65" s="10" cm="1">
+        <f t="array" ref="E65">_xlfn.XLOOKUP($A65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(E$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="F65" s="10" cm="1">
+        <f t="array" ref="F65">_xlfn.XLOOKUP($A65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(F$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="G65" s="10" cm="1">
+        <f t="array" ref="G65">_xlfn.XLOOKUP($A65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -5521,8 +5562,20 @@
         <f t="shared" ref="D66:D70" si="16">_xlfn.XLOOKUP($A66, $A$2:$A$52, $N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E66" s="10" cm="1">
+        <f t="array" ref="E66">_xlfn.XLOOKUP($A66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(E$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="10" cm="1">
+        <f t="array" ref="F66">_xlfn.XLOOKUP($A66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(F$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="10" cm="1">
+        <f t="array" ref="G66">_xlfn.XLOOKUP($A66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -5538,8 +5591,20 @@
         <f t="shared" si="16"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E67" s="10" cm="1">
+        <f t="array" ref="E67">_xlfn.XLOOKUP($A67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(E$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="F67" s="10" cm="1">
+        <f t="array" ref="F67">_xlfn.XLOOKUP($A67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(F$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="G67" s="10" cm="1">
+        <f t="array" ref="G67">_xlfn.XLOOKUP($A67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -5555,8 +5620,20 @@
         <f t="shared" si="16"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E68" s="10" cm="1">
+        <f t="array" ref="E68">_xlfn.XLOOKUP($A68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(E$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="F68" s="10" cm="1">
+        <f t="array" ref="F68">_xlfn.XLOOKUP($A68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(F$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="G68" s="10" cm="1">
+        <f t="array" ref="G68">_xlfn.XLOOKUP($A68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -5572,8 +5649,20 @@
         <f t="shared" si="16"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E69" s="10" cm="1">
+        <f t="array" ref="E69">_xlfn.XLOOKUP($A69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(E$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="F69" s="10" cm="1">
+        <f t="array" ref="F69">_xlfn.XLOOKUP($A69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(F$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="G69" s="10" cm="1">
+        <f t="array" ref="G69">_xlfn.XLOOKUP($A69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -5589,6 +5678,18 @@
         <f t="shared" si="16"/>
         <v>-82077.349999999627</v>
       </c>
+      <c r="E70" s="10" cm="1">
+        <f t="array" ref="E70">_xlfn.XLOOKUP($A70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(E$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="F70" s="10" cm="1">
+        <f t="array" ref="F70">_xlfn.XLOOKUP($A70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(F$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="G70" s="10" cm="1">
+        <f t="array" ref="G70">_xlfn.XLOOKUP($A70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-82077.349999999627</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
@@ -5901,24 +6002,60 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
       <c r="C91" s="5"/>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP(D$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
       <c r="E91" s="5"/>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP(F$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>74</v>
       </c>
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP(B$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
       <c r="C92" s="5"/>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP(D$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
       <c r="E92" s="5"/>
+      <c r="F92" t="str">
+        <f>_xlfn.XLOOKUP(F$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Office of Family Safety</v>
+      </c>
       <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>75</v>
       </c>
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP(B$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
       <c r="C93" s="5"/>
+      <c r="D93" t="str">
+        <f>_xlfn.XLOOKUP(D$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
       <c r="E93" s="5"/>
+      <c r="F93" t="str">
+        <f>_xlfn.XLOOKUP(F$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Election Commission</v>
+      </c>
       <c r="G93" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>